<commit_message>
update 23Q4 details and ready for 24Q1 new season
</commit_message>
<xml_diff>
--- a/2023_Q4/2023-Q4_羽球季打費用明細.xlsx
+++ b/2023_Q4/2023-Q4_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DFE91B-BA80-4565-838D-BB317AE37F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262471F2-DC44-4B24-8D05-B04A72C8B10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-106" yWindow="-106" windowWidth="22828" windowHeight="12209" tabRatio="738" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-86" yWindow="0" windowWidth="11143" windowHeight="11709" tabRatio="738" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q4收支明細" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,19 +58,83 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>=SUM(B2:C16)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023/09/14 更新餘額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>現金 2023Q3結餘</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2023Q4 場地費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 偉群 07/24臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Ivy 季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Richart 24891 @Marco 季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @夜市喧 季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @鉉竣季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Frank 季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉帳 28838 @蕭鎮豪 季打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Frank友 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 鎮豪友 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Frank友、Unie、CY 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 彥杰 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 彥杰、鎮豪友、帆船 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 鎮豪友*2 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蝦皮購入 VOLAR-10 羽球三桶 $380*3+$29(運費)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINEPAY 靖懷 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINEPAY/現金 靖懷/帆船 臨打費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/12/04 更新餘額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=SUM(B2:C24)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -79,8 +143,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -178,40 +242,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
@@ -539,19 +603,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCCEF2F-70B8-4CD5-8F32-AA2B6924B187}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.15234375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.15234375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,103 +631,264 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
+        <v>45183</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3690</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="8">
         <v>45180</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B3" s="9">
         <v>-8560</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>45180</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1430</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8">
-        <v>45183</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10">
-        <v>3690</v>
-      </c>
-      <c r="D3" s="11" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="8">
+        <v>45187</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10">
+        <v>1430</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="5">
+        <v>45187</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1430</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="8">
+        <v>45187</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10">
+        <v>1430</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="5">
+        <v>45187</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1430</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="8">
+        <v>45187</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10">
+        <v>1430</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="5">
+        <v>45187</v>
+      </c>
+      <c r="C10" s="7">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="8"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="8">
+        <v>45201</v>
+      </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="8"/>
+      <c r="C11" s="10">
+        <v>150</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="5">
+        <v>45215</v>
+      </c>
+      <c r="C12" s="7">
+        <v>150</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="8">
+        <v>45222</v>
+      </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
+      <c r="C13" s="10">
+        <v>450</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="5">
+        <v>45229</v>
+      </c>
+      <c r="C14" s="7">
+        <v>150</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="8">
+        <v>45236</v>
+      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="12" t="s">
+      <c r="C15" s="10">
+        <v>450</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="5">
+        <v>45243</v>
+      </c>
+      <c r="C16" s="7">
+        <v>300</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="8">
+        <v>45250</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10">
+        <v>150</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="5">
+        <v>45255</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-1169</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="8">
+        <v>45257</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10">
+        <v>150</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="5">
+        <v>45264</v>
+      </c>
+      <c r="C20" s="7">
+        <v>300</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.3" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13">
-        <f>SUM(B2:C16)</f>
-        <v>-4870</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D18" s="15" t="s">
-        <v>6</v>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13">
+        <f>SUM(B2:C24)</f>
+        <v>4941</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D26" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>